<commit_message>
Committed the previous code to the repository
</commit_message>
<xml_diff>
--- a/updated_portfolio.xlsx
+++ b/updated_portfolio.xlsx
@@ -523,23 +523,23 @@
         <v>4781.04</v>
       </c>
       <c r="G2" t="n">
-        <v>705.85</v>
+        <v>682.95</v>
       </c>
       <c r="H2" t="n">
-        <v>8470.200000000001</v>
+        <v>8195.400000000001</v>
       </c>
       <c r="I2" t="n">
-        <v>3689.160000000001</v>
+        <v>3414.360000000001</v>
       </c>
       <c r="J2" t="n">
-        <v>77.16229104964611</v>
+        <v>71.41458762110339</v>
       </c>
       <c r="K2" t="n">
-        <v>-0.4583274573402905</v>
+        <v>-1.910233393177731</v>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>2025-09-11 10:20:12</t>
+          <t>2025-09-24 10:20:17</t>
         </is>
       </c>
     </row>
@@ -569,23 +569,23 @@
         <v>9412.82</v>
       </c>
       <c r="G3" t="n">
-        <v>169.41</v>
+        <v>172.66</v>
       </c>
       <c r="H3" t="n">
-        <v>9825.780000000001</v>
+        <v>10014.28</v>
       </c>
       <c r="I3" t="n">
-        <v>412.9600000000009</v>
+        <v>601.4600000000009</v>
       </c>
       <c r="J3" t="n">
-        <v>4.387208084293559</v>
+        <v>6.389796044118564</v>
       </c>
       <c r="K3" t="n">
-        <v>-0.01180428495544486</v>
+        <v>0.7410000583464673</v>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>2025-09-11 10:20:12</t>
+          <t>2025-09-24 10:20:17</t>
         </is>
       </c>
     </row>
@@ -615,23 +615,23 @@
         <v>1489.48</v>
       </c>
       <c r="G4" t="n">
-        <v>1509.7</v>
+        <v>1494.6</v>
       </c>
       <c r="H4" t="n">
-        <v>1509.7</v>
+        <v>1494.6</v>
       </c>
       <c r="I4" t="n">
-        <v>20.22000000000003</v>
+        <v>5.119999999999891</v>
       </c>
       <c r="J4" t="n">
-        <v>1.357520745495074</v>
+        <v>0.3437441254665985</v>
       </c>
       <c r="K4" t="n">
-        <v>-1.494192874853182</v>
+        <v>-0.3267755918639607</v>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>2025-09-11 10:20:12</t>
+          <t>2025-09-24 10:20:17</t>
         </is>
       </c>
     </row>
@@ -661,23 +661,23 @@
         <v>42672</v>
       </c>
       <c r="G5" t="n">
-        <v>877.1</v>
+        <v>894.25</v>
       </c>
       <c r="H5" t="n">
-        <v>42100.8</v>
+        <v>42924</v>
       </c>
       <c r="I5" t="n">
-        <v>-571.1999999999971</v>
+        <v>252</v>
       </c>
       <c r="J5" t="n">
-        <v>-1.338582677165348</v>
+        <v>0.5905511811023622</v>
       </c>
       <c r="K5" t="n">
-        <v>-0.06266735031048305</v>
+        <v>-1.13322277501382</v>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>2025-09-11 10:20:12</t>
+          <t>2025-09-24 10:20:17</t>
         </is>
       </c>
     </row>
@@ -707,23 +707,23 @@
         <v>3683.25</v>
       </c>
       <c r="G6" t="n">
-        <v>437.7</v>
+        <v>448.45</v>
       </c>
       <c r="H6" t="n">
-        <v>6565.5</v>
+        <v>6726.75</v>
       </c>
       <c r="I6" t="n">
-        <v>2882.25</v>
+        <v>3043.5</v>
       </c>
       <c r="J6" t="n">
-        <v>78.25290164935859</v>
+        <v>82.63082875178172</v>
       </c>
       <c r="K6" t="n">
-        <v>0.9222965183306434</v>
+        <v>-2.181262951248773</v>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>2025-09-11 10:20:12</t>
+          <t>2025-09-24 10:20:17</t>
         </is>
       </c>
     </row>
@@ -753,23 +753,23 @@
         <v>12777.93</v>
       </c>
       <c r="G7" t="n">
-        <v>422.7</v>
+        <v>399.6</v>
       </c>
       <c r="H7" t="n">
-        <v>13949.1</v>
+        <v>13186.8</v>
       </c>
       <c r="I7" t="n">
-        <v>1171.170000000002</v>
+        <v>408.8700000000026</v>
       </c>
       <c r="J7" t="n">
-        <v>9.165569071046734</v>
+        <v>3.199814054389112</v>
       </c>
       <c r="K7" t="n">
-        <v>0.1065719360568357</v>
+        <v>-1.052370929800668</v>
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>2025-09-11 10:20:12</t>
+          <t>2025-09-24 10:20:17</t>
         </is>
       </c>
     </row>
@@ -799,23 +799,23 @@
         <v>10452.4</v>
       </c>
       <c r="G8" t="n">
-        <v>388.1</v>
+        <v>390.3</v>
       </c>
       <c r="H8" t="n">
-        <v>15524</v>
+        <v>15612</v>
       </c>
       <c r="I8" t="n">
-        <v>5071.6</v>
+        <v>5159.6</v>
       </c>
       <c r="J8" t="n">
-        <v>48.52091385710459</v>
+        <v>49.36282576250431</v>
       </c>
       <c r="K8" t="n">
-        <v>0.4139715394566683</v>
+        <v>-1.264862130027827</v>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>2025-09-11 10:20:12</t>
+          <t>2025-09-24 10:20:17</t>
         </is>
       </c>
     </row>
@@ -845,23 +845,23 @@
         <v>947.96</v>
       </c>
       <c r="G9" t="n">
-        <v>29.09</v>
+        <v>29.56</v>
       </c>
       <c r="H9" t="n">
-        <v>756.34</v>
+        <v>768.5599999999999</v>
       </c>
       <c r="I9" t="n">
-        <v>-191.62</v>
+        <v>-179.4000000000001</v>
       </c>
       <c r="J9" t="n">
-        <v>-20.21393307734504</v>
+        <v>-18.92484914975316</v>
       </c>
       <c r="K9" t="n">
-        <v>-0.2400548696845003</v>
+        <v>-2.602965403624391</v>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>2025-09-11 10:20:12</t>
+          <t>2025-09-24 10:20:17</t>
         </is>
       </c>
     </row>
@@ -891,23 +891,23 @@
         <v>762.4</v>
       </c>
       <c r="G10" t="n">
-        <v>233.76</v>
+        <v>238.52</v>
       </c>
       <c r="H10" t="n">
-        <v>1168.8</v>
+        <v>1192.6</v>
       </c>
       <c r="I10" t="n">
-        <v>406.4</v>
+        <v>430.2000000000002</v>
       </c>
       <c r="J10" t="n">
-        <v>53.30535152151101</v>
+        <v>56.42707240293812</v>
       </c>
       <c r="K10" t="n">
-        <v>0.8716665228272986</v>
+        <v>0.4421611150882265</v>
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>2025-09-11 10:20:12</t>
+          <t>2025-09-24 10:20:17</t>
         </is>
       </c>
     </row>
@@ -937,23 +937,23 @@
         <v>4550.45</v>
       </c>
       <c r="G11" t="n">
-        <v>968.25</v>
+        <v>964.15</v>
       </c>
       <c r="H11" t="n">
-        <v>4841.25</v>
+        <v>4820.75</v>
       </c>
       <c r="I11" t="n">
-        <v>290.8000000000002</v>
+        <v>270.3000000000002</v>
       </c>
       <c r="J11" t="n">
-        <v>6.390576756145001</v>
+        <v>5.940071861024738</v>
       </c>
       <c r="K11" t="n">
-        <v>2.46031746031746</v>
+        <v>-1.006211817855133</v>
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>2025-09-11 10:20:12</t>
+          <t>2025-09-24 10:20:17</t>
         </is>
       </c>
     </row>
@@ -983,23 +983,23 @@
         <v>4867.200000000001</v>
       </c>
       <c r="G12" t="n">
-        <v>331.05</v>
+        <v>347.6</v>
       </c>
       <c r="H12" t="n">
-        <v>4965.75</v>
+        <v>5214</v>
       </c>
       <c r="I12" t="n">
-        <v>98.54999999999927</v>
+        <v>346.7999999999993</v>
       </c>
       <c r="J12" t="n">
-        <v>2.02477810650886</v>
+        <v>7.125246548323455</v>
       </c>
       <c r="K12" t="n">
-        <v>1.658222017503465</v>
+        <v>2.476415094339633</v>
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>2025-09-11 10:20:12</t>
+          <t>2025-09-24 10:20:17</t>
         </is>
       </c>
     </row>
@@ -1029,23 +1029,23 @@
         <v>3716.9</v>
       </c>
       <c r="G13" t="n">
-        <v>719.7</v>
+        <v>715.45</v>
       </c>
       <c r="H13" t="n">
-        <v>3598.5</v>
+        <v>3577.25</v>
       </c>
       <c r="I13" t="n">
-        <v>-118.4000000000001</v>
+        <v>-139.6500000000001</v>
       </c>
       <c r="J13" t="n">
-        <v>-3.18545024079206</v>
+        <v>-3.757163227420703</v>
       </c>
       <c r="K13" t="n">
-        <v>0.1600445341312492</v>
+        <v>-1.602255535689723</v>
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>2025-09-11 10:20:12</t>
+          <t>2025-09-24 10:20:17</t>
         </is>
       </c>
     </row>
@@ -1075,23 +1075,23 @@
         <v>13152.8</v>
       </c>
       <c r="G14" t="n">
-        <v>143.42</v>
+        <v>140.41</v>
       </c>
       <c r="H14" t="n">
-        <v>11473.6</v>
+        <v>11232.8</v>
       </c>
       <c r="I14" t="n">
-        <v>-1679.200000000001</v>
+        <v>-1920</v>
       </c>
       <c r="J14" t="n">
-        <v>-12.76686332948118</v>
+        <v>-14.59765221093607</v>
       </c>
       <c r="K14" t="n">
-        <v>-0.9119801022523294</v>
+        <v>-3.888014237798622</v>
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>2025-09-11 10:20:12</t>
+          <t>2025-09-24 10:20:17</t>
         </is>
       </c>
     </row>
@@ -1121,23 +1121,23 @@
         <v>3096.78</v>
       </c>
       <c r="G15" t="n">
-        <v>1467.7</v>
+        <v>1442.3</v>
       </c>
       <c r="H15" t="n">
-        <v>4403.1</v>
+        <v>4326.9</v>
       </c>
       <c r="I15" t="n">
-        <v>1306.320000000001</v>
+        <v>1230.12</v>
       </c>
       <c r="J15" t="n">
-        <v>42.18317090655457</v>
+        <v>39.72255052021777</v>
       </c>
       <c r="K15" t="n">
-        <v>0.2595805724434698</v>
+        <v>0.1666782415445422</v>
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>2025-09-11 10:20:12</t>
+          <t>2025-09-24 10:20:17</t>
         </is>
       </c>
     </row>
@@ -1190,20 +1190,20 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-09-11</t>
+          <t>2025-09-24</t>
         </is>
       </c>
       <c r="B2" t="n">
         <v>116363.41</v>
       </c>
       <c r="C2" t="n">
-        <v>129152.42</v>
+        <v>129286.69</v>
       </c>
       <c r="D2" t="n">
-        <v>12789.01000000002</v>
+        <v>12923.28000000001</v>
       </c>
       <c r="E2" t="n">
-        <v>10.99057684885655</v>
+        <v>11.10596535457324</v>
       </c>
     </row>
   </sheetData>
@@ -1255,20 +1255,20 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-09-11</t>
+          <t>2025-09-24</t>
         </is>
       </c>
       <c r="B2" t="n">
         <v>116363.41</v>
       </c>
       <c r="C2" t="n">
-        <v>129152.42</v>
+        <v>129286.69</v>
       </c>
       <c r="D2" t="n">
-        <v>12789.01000000002</v>
+        <v>12923.28000000001</v>
       </c>
       <c r="E2" t="n">
-        <v>10.99057684885655</v>
+        <v>11.10596535457324</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Pushed recent changes and updates into the repository
</commit_message>
<xml_diff>
--- a/updated_portfolio.xlsx
+++ b/updated_portfolio.xlsx
@@ -522,24 +522,16 @@
       <c r="F2" t="n">
         <v>4781.04</v>
       </c>
-      <c r="G2" t="n">
-        <v>682.95</v>
-      </c>
-      <c r="H2" t="n">
-        <v>8195.400000000001</v>
-      </c>
-      <c r="I2" t="n">
-        <v>3414.360000000001</v>
-      </c>
-      <c r="J2" t="n">
-        <v>71.41458762110339</v>
-      </c>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
       <c r="K2" t="n">
-        <v>-1.910233393177731</v>
+        <v>0</v>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>2025-09-24 10:20:17</t>
+          <t>2025-11-18 10:20:13</t>
         </is>
       </c>
     </row>
@@ -569,23 +561,23 @@
         <v>9412.82</v>
       </c>
       <c r="G3" t="n">
-        <v>172.66</v>
+        <v>172.45</v>
       </c>
       <c r="H3" t="n">
-        <v>10014.28</v>
+        <v>10002.1</v>
       </c>
       <c r="I3" t="n">
-        <v>601.4600000000009</v>
+        <v>589.2799999999988</v>
       </c>
       <c r="J3" t="n">
-        <v>6.389796044118564</v>
+        <v>6.26039805286831</v>
       </c>
       <c r="K3" t="n">
-        <v>0.7410000583464673</v>
+        <v>-0.4157764046890332</v>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>2025-09-24 10:20:17</t>
+          <t>2025-11-18 10:20:13</t>
         </is>
       </c>
     </row>
@@ -615,23 +607,23 @@
         <v>1489.48</v>
       </c>
       <c r="G4" t="n">
-        <v>1494.6</v>
+        <v>1486.4</v>
       </c>
       <c r="H4" t="n">
-        <v>1494.6</v>
+        <v>1486.4</v>
       </c>
       <c r="I4" t="n">
-        <v>5.119999999999891</v>
+        <v>-3.079999999999927</v>
       </c>
       <c r="J4" t="n">
-        <v>0.3437441254665985</v>
+        <v>-0.2067835754760002</v>
       </c>
       <c r="K4" t="n">
-        <v>-0.3267755918639607</v>
+        <v>-1.406208543380195</v>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>2025-09-24 10:20:17</t>
+          <t>2025-11-18 10:20:13</t>
         </is>
       </c>
     </row>
@@ -661,23 +653,23 @@
         <v>42672</v>
       </c>
       <c r="G5" t="n">
-        <v>894.25</v>
+        <v>915.5</v>
       </c>
       <c r="H5" t="n">
-        <v>42924</v>
+        <v>43944</v>
       </c>
       <c r="I5" t="n">
-        <v>252</v>
+        <v>1272</v>
       </c>
       <c r="J5" t="n">
-        <v>0.5905511811023622</v>
+        <v>2.98087739032621</v>
       </c>
       <c r="K5" t="n">
-        <v>-1.13322277501382</v>
+        <v>0.01638717430490821</v>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>2025-09-24 10:20:17</t>
+          <t>2025-11-18 10:20:13</t>
         </is>
       </c>
     </row>
@@ -707,23 +699,23 @@
         <v>3683.25</v>
       </c>
       <c r="G6" t="n">
-        <v>448.45</v>
+        <v>510.7</v>
       </c>
       <c r="H6" t="n">
-        <v>6726.75</v>
+        <v>7660.5</v>
       </c>
       <c r="I6" t="n">
-        <v>3043.5</v>
+        <v>3977.25</v>
       </c>
       <c r="J6" t="n">
-        <v>82.63082875178172</v>
+        <v>107.9820810425575</v>
       </c>
       <c r="K6" t="n">
-        <v>-2.181262951248773</v>
+        <v>-1.939324116743465</v>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>2025-09-24 10:20:17</t>
+          <t>2025-11-18 10:20:13</t>
         </is>
       </c>
     </row>
@@ -753,23 +745,23 @@
         <v>12777.93</v>
       </c>
       <c r="G7" t="n">
-        <v>399.6</v>
+        <v>381.5</v>
       </c>
       <c r="H7" t="n">
-        <v>13186.8</v>
+        <v>12589.5</v>
       </c>
       <c r="I7" t="n">
-        <v>408.8700000000026</v>
+        <v>-188.4299999999985</v>
       </c>
       <c r="J7" t="n">
-        <v>3.199814054389112</v>
+        <v>-1.474651997624016</v>
       </c>
       <c r="K7" t="n">
-        <v>-1.052370929800668</v>
+        <v>-0.3135615364515257</v>
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>2025-09-24 10:20:17</t>
+          <t>2025-11-18 10:20:13</t>
         </is>
       </c>
     </row>
@@ -799,23 +791,23 @@
         <v>10452.4</v>
       </c>
       <c r="G8" t="n">
-        <v>390.3</v>
+        <v>386.25</v>
       </c>
       <c r="H8" t="n">
-        <v>15612</v>
+        <v>15450</v>
       </c>
       <c r="I8" t="n">
-        <v>5159.6</v>
+        <v>4997.6</v>
       </c>
       <c r="J8" t="n">
-        <v>49.36282576250431</v>
+        <v>47.81294248210938</v>
       </c>
       <c r="K8" t="n">
-        <v>-1.264862130027827</v>
+        <v>-1.654996817313813</v>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>2025-09-24 10:20:17</t>
+          <t>2025-11-18 10:20:13</t>
         </is>
       </c>
     </row>
@@ -845,23 +837,23 @@
         <v>947.96</v>
       </c>
       <c r="G9" t="n">
-        <v>29.56</v>
+        <v>28.38</v>
       </c>
       <c r="H9" t="n">
-        <v>768.5599999999999</v>
+        <v>737.88</v>
       </c>
       <c r="I9" t="n">
-        <v>-179.4000000000001</v>
+        <v>-210.08</v>
       </c>
       <c r="J9" t="n">
-        <v>-18.92484914975316</v>
+        <v>-22.16127262753703</v>
       </c>
       <c r="K9" t="n">
-        <v>-2.602965403624391</v>
+        <v>-0.2460456942003525</v>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>2025-09-24 10:20:17</t>
+          <t>2025-11-18 10:20:13</t>
         </is>
       </c>
     </row>
@@ -891,23 +883,23 @@
         <v>762.4</v>
       </c>
       <c r="G10" t="n">
-        <v>238.52</v>
+        <v>246.95</v>
       </c>
       <c r="H10" t="n">
-        <v>1192.6</v>
+        <v>1234.75</v>
       </c>
       <c r="I10" t="n">
-        <v>430.2000000000002</v>
+        <v>472.35</v>
       </c>
       <c r="J10" t="n">
-        <v>56.42707240293812</v>
+        <v>61.95566631689402</v>
       </c>
       <c r="K10" t="n">
-        <v>0.4421611150882265</v>
+        <v>-0.443458980044355</v>
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>2025-09-24 10:20:17</t>
+          <t>2025-11-18 10:20:13</t>
         </is>
       </c>
     </row>
@@ -937,23 +929,23 @@
         <v>4550.45</v>
       </c>
       <c r="G11" t="n">
-        <v>964.15</v>
+        <v>826.7</v>
       </c>
       <c r="H11" t="n">
-        <v>4820.75</v>
+        <v>4133.5</v>
       </c>
       <c r="I11" t="n">
-        <v>270.3000000000002</v>
+        <v>-416.9499999999998</v>
       </c>
       <c r="J11" t="n">
-        <v>5.940071861024738</v>
+        <v>-9.162830049775293</v>
       </c>
       <c r="K11" t="n">
-        <v>-1.006211817855133</v>
+        <v>-0.9287554676733176</v>
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>2025-09-24 10:20:17</t>
+          <t>2025-11-18 10:20:13</t>
         </is>
       </c>
     </row>
@@ -983,23 +975,23 @@
         <v>4867.200000000001</v>
       </c>
       <c r="G12" t="n">
-        <v>347.6</v>
+        <v>328.45</v>
       </c>
       <c r="H12" t="n">
-        <v>5214</v>
+        <v>4926.75</v>
       </c>
       <c r="I12" t="n">
-        <v>346.7999999999993</v>
+        <v>59.54999999999927</v>
       </c>
       <c r="J12" t="n">
-        <v>7.125246548323455</v>
+        <v>1.223496055226809</v>
       </c>
       <c r="K12" t="n">
-        <v>2.476415094339633</v>
+        <v>-0.5299818291944276</v>
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>2025-09-24 10:20:17</t>
+          <t>2025-11-18 10:20:13</t>
         </is>
       </c>
     </row>
@@ -1029,23 +1021,23 @@
         <v>3716.9</v>
       </c>
       <c r="G13" t="n">
-        <v>715.45</v>
+        <v>703.8</v>
       </c>
       <c r="H13" t="n">
-        <v>3577.25</v>
+        <v>3519</v>
       </c>
       <c r="I13" t="n">
-        <v>-139.6500000000001</v>
+        <v>-197.9000000000001</v>
       </c>
       <c r="J13" t="n">
-        <v>-3.757163227420703</v>
+        <v>-5.324329414296862</v>
       </c>
       <c r="K13" t="n">
-        <v>-1.602255535689723</v>
+        <v>-1.297244232522264</v>
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>2025-09-24 10:20:17</t>
+          <t>2025-11-18 10:20:13</t>
         </is>
       </c>
     </row>
@@ -1075,23 +1067,23 @@
         <v>13152.8</v>
       </c>
       <c r="G14" t="n">
-        <v>140.41</v>
+        <v>136.65</v>
       </c>
       <c r="H14" t="n">
-        <v>11232.8</v>
+        <v>10932</v>
       </c>
       <c r="I14" t="n">
-        <v>-1920</v>
+        <v>-2220.799999999999</v>
       </c>
       <c r="J14" t="n">
-        <v>-14.59765221093607</v>
+        <v>-16.88461772398272</v>
       </c>
       <c r="K14" t="n">
-        <v>-3.888014237798622</v>
+        <v>-0.6543075245365362</v>
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>2025-09-24 10:20:17</t>
+          <t>2025-11-18 10:20:13</t>
         </is>
       </c>
     </row>
@@ -1121,23 +1113,23 @@
         <v>3096.78</v>
       </c>
       <c r="G15" t="n">
-        <v>1442.3</v>
+        <v>1595.2</v>
       </c>
       <c r="H15" t="n">
-        <v>4326.9</v>
+        <v>4785.6</v>
       </c>
       <c r="I15" t="n">
-        <v>1230.12</v>
+        <v>1688.820000000001</v>
       </c>
       <c r="J15" t="n">
-        <v>39.72255052021777</v>
+        <v>54.5347102474183</v>
       </c>
       <c r="K15" t="n">
-        <v>0.1666782415445422</v>
+        <v>-0.6972111553784888</v>
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>2025-09-24 10:20:17</t>
+          <t>2025-11-18 10:20:13</t>
         </is>
       </c>
     </row>
@@ -1190,20 +1182,20 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-11-18</t>
         </is>
       </c>
       <c r="B2" t="n">
         <v>116363.41</v>
       </c>
       <c r="C2" t="n">
-        <v>129286.69</v>
+        <v>121401.98</v>
       </c>
       <c r="D2" t="n">
-        <v>12923.28000000001</v>
+        <v>5038.570000000022</v>
       </c>
       <c r="E2" t="n">
-        <v>11.10596535457324</v>
+        <v>4.330029517010564</v>
       </c>
     </row>
   </sheetData>
@@ -1255,20 +1247,20 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-11-18</t>
         </is>
       </c>
       <c r="B2" t="n">
         <v>116363.41</v>
       </c>
       <c r="C2" t="n">
-        <v>129286.69</v>
+        <v>121401.98</v>
       </c>
       <c r="D2" t="n">
-        <v>12923.28000000001</v>
+        <v>5038.570000000022</v>
       </c>
       <c r="E2" t="n">
-        <v>11.10596535457324</v>
+        <v>4.330029517010564</v>
       </c>
     </row>
   </sheetData>

</xml_diff>